<commit_message>
changed the lbb weights to multiples of 147 to match the size of IBTC data that was made of 147 observations(dont know if that makes much sense but it makes the plots look right). Also changed the date cutoff to 2024-01-11 untill 2024-06-05.
</commit_message>
<xml_diff>
--- a/statistics_summary.xlsx
+++ b/statistics_summary.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>BTC</t>
+          <t>IBTC</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -466,14 +466,20 @@
           <t>Mean</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="n">
+        <v>34.02081627210884</v>
+      </c>
       <c r="C2" t="n">
-        <v>113103.5573758894</v>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
+        <v>127376.8027210884</v>
+      </c>
+      <c r="D2" t="n">
+        <v>9875.46084602721</v>
+      </c>
+      <c r="E2" t="n">
+        <v>7.855714285714286</v>
+      </c>
       <c r="F2" t="n">
-        <v>239.249896064683</v>
+        <v>285.7742180816327</v>
       </c>
     </row>
     <row r="3">
@@ -482,14 +488,20 @@
           <t>Median</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="n">
+        <v>36.209999</v>
+      </c>
       <c r="C3" t="n">
-        <v>113416</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
+        <v>127668</v>
+      </c>
+      <c r="D3" t="n">
+        <v>9886.252229</v>
+      </c>
+      <c r="E3" t="n">
+        <v>7.91</v>
+      </c>
       <c r="F3" t="n">
-        <v>235.050003</v>
+        <v>288.290009</v>
       </c>
     </row>
     <row r="4">
@@ -498,14 +510,20 @@
           <t>Standard Deviation</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="n">
+        <v>5.842908680803125</v>
+      </c>
       <c r="C4" t="n">
-        <v>10552.31956480709</v>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
+        <v>2017.562372534595</v>
+      </c>
+      <c r="D4" t="n">
+        <v>38.76511435206717</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.2591115117284527</v>
+      </c>
       <c r="F4" t="n">
-        <v>31.58397884229408</v>
+        <v>12.97404173256524</v>
       </c>
     </row>
     <row r="5">
@@ -514,14 +532,20 @@
           <t>Kurtosis</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
+      <c r="B5" t="n">
+        <v>-1.017277626065159</v>
+      </c>
       <c r="C5" t="n">
-        <v>0.2057875950431232</v>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+        <v>0.8240942329896561</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-0.2770808927941548</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-0.4171455961159491</v>
+      </c>
       <c r="F5" t="n">
-        <v>0.07015955917845096</v>
+        <v>-0.4368381318723622</v>
       </c>
     </row>
     <row r="6">
@@ -530,14 +554,20 @@
           <t>Skewness</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
+      <c r="B6" t="n">
+        <v>-0.6936905131393687</v>
+      </c>
       <c r="C6" t="n">
-        <v>-0.4482033967560713</v>
-      </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
+        <v>-0.805890693663089</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-0.6165237100922017</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-0.5060570587828281</v>
+      </c>
       <c r="F6" t="n">
-        <v>0.3471818314018826</v>
+        <v>-0.2494028448025493</v>
       </c>
     </row>
     <row r="7">
@@ -547,19 +577,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.3848440890582389</v>
+        <v>0.06199446552504129</v>
       </c>
       <c r="C7" t="n">
-        <v>0.08859524126012688</v>
+        <v>0.09843999638032346</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4875228494544159</v>
+        <v>0.09308118403278205</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1846783410689072</v>
+        <v>0.0980346371114356</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0908307938120707</v>
+        <v>0.1000914157361388</v>
       </c>
     </row>
     <row r="8">
@@ -569,19 +599,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1.205609030371254</v>
+        <v>0.1869231013248247</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2210310604434397</v>
+        <v>0.236840330337551</v>
       </c>
       <c r="D8" t="n">
-        <v>1.438652799605457</v>
+        <v>0.2260385773870736</v>
       </c>
       <c r="E8" t="n">
-        <v>0.4975315722297103</v>
+        <v>0.2342371191902062</v>
       </c>
       <c r="F8" t="n">
-        <v>0.2326786936433567</v>
+        <v>0.2965468887295143</v>
       </c>
     </row>
     <row r="9">
@@ -591,19 +621,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.1792350586869841</v>
+        <v>0.8750713642002167</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8675641808166873</v>
+        <v>0.8615996660427724</v>
       </c>
       <c r="D9" t="n">
-        <v>0.04887004984895887</v>
+        <v>0.8670426066457084</v>
       </c>
       <c r="E9" t="n">
-        <v>0.6871467688391971</v>
+        <v>0.8637975179212295</v>
       </c>
       <c r="F9" t="n">
-        <v>0.858152100168714</v>
+        <v>0.8035445270066246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edited some graphical things mostly
</commit_message>
<xml_diff>
--- a/statistics_summary.xlsx
+++ b/statistics_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,25 +436,20 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>IBTC</t>
+          <t>IBOVESPA</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>IBOVESPA</t>
+          <t>IMA-B</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>IMA-B</t>
+          <t>SCBTG</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>SCBTG</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>S&amp;P 500</t>
         </is>
@@ -467,19 +462,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>34.02081627210884</v>
+        <v>114014.0912738215</v>
       </c>
       <c r="C2" t="n">
-        <v>127376.8027210884</v>
+        <v>8858.345973007021</v>
       </c>
       <c r="D2" t="n">
-        <v>9875.46084602721</v>
+        <v>7.977432296890672</v>
       </c>
       <c r="E2" t="n">
-        <v>7.855714285714286</v>
-      </c>
-      <c r="F2" t="n">
-        <v>285.7742180816327</v>
+        <v>246.6238513971916</v>
       </c>
     </row>
     <row r="3">
@@ -489,19 +481,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>36.209999</v>
+        <v>112764</v>
       </c>
       <c r="C3" t="n">
-        <v>127668</v>
+        <v>8569.517189</v>
       </c>
       <c r="D3" t="n">
-        <v>9886.252229</v>
+        <v>8.039999999999999</v>
       </c>
       <c r="E3" t="n">
-        <v>7.91</v>
-      </c>
-      <c r="F3" t="n">
-        <v>288.290009</v>
+        <v>238.789993</v>
       </c>
     </row>
     <row r="4">
@@ -511,19 +500,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5.842908680803125</v>
+        <v>8847.243905469244</v>
       </c>
       <c r="C4" t="n">
-        <v>2017.562372534595</v>
+        <v>700.844902350853</v>
       </c>
       <c r="D4" t="n">
-        <v>38.76511435206717</v>
+        <v>0.745963949075289</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2591115117284527</v>
-      </c>
-      <c r="F4" t="n">
-        <v>12.97404173256524</v>
+        <v>25.03584273367861</v>
       </c>
     </row>
     <row r="5">
@@ -533,19 +519,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-1.017277626065159</v>
+        <v>-0.711850269504962</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8240942329896561</v>
+        <v>-1.451583380115703</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.2770808927941548</v>
+        <v>0.9528817755822936</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.4171455961159491</v>
-      </c>
-      <c r="F5" t="n">
-        <v>-0.4368381318723622</v>
+        <v>-0.5655566533230973</v>
       </c>
     </row>
     <row r="6">
@@ -555,19 +538,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.6936905131393687</v>
+        <v>0.3556782972634858</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.805890693663089</v>
+        <v>0.210039751158321</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.6165237100922017</v>
+        <v>0.5232456205924026</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.5060570587828281</v>
-      </c>
-      <c r="F6" t="n">
-        <v>-0.2494028448025493</v>
+        <v>0.7397614525688554</v>
       </c>
     </row>
     <row r="7">
@@ -577,19 +557,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.06199446552504129</v>
+        <v>0.1003180021900583</v>
       </c>
       <c r="C7" t="n">
-        <v>0.09843999638032346</v>
+        <v>0.1089998067752257</v>
       </c>
       <c r="D7" t="n">
-        <v>0.09308118403278205</v>
+        <v>0.1127085498772781</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0980346371114356</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.1000914157361388</v>
+        <v>0.09133581486054189</v>
       </c>
     </row>
     <row r="8">
@@ -599,19 +576,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1869231013248247</v>
+        <v>0.2441202301271639</v>
       </c>
       <c r="C8" t="n">
-        <v>0.236840330337551</v>
+        <v>0.2861911670287034</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2260385773870736</v>
+        <v>0.2740876642375576</v>
       </c>
       <c r="E8" t="n">
-        <v>0.2342371191902062</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.2965468887295143</v>
+        <v>0.2301067906714883</v>
       </c>
     </row>
     <row r="9">
@@ -621,19 +595,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.8750713642002167</v>
+        <v>0.8561977720628944</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8615996660427724</v>
+        <v>0.8228086397465223</v>
       </c>
       <c r="D9" t="n">
-        <v>0.8670426066457084</v>
+        <v>0.8386208856397205</v>
       </c>
       <c r="E9" t="n">
-        <v>0.8637975179212295</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.8035445270066246</v>
+        <v>0.8612290241890536</v>
       </c>
     </row>
   </sheetData>

</xml_diff>